<commit_message>
Changed sample primary key to sample id instead of lane id
</commit_message>
<xml_diff>
--- a/e2e/fixtures/test_committable.xlsx
+++ b/e2e/fixtures/test_committable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/km22/Documents/git_projects/monocle/e2e/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kp11/workspace/applications/monocle/e2e/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81EC4F6-AFEE-744F-AD77-ADAAE95CBD63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B039AD-65B1-214C-AE64-1BF674D5F24B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="10000" windowWidth="17160" windowHeight="16640" xr2:uid="{44B2F2F3-C1F6-DD4A-8564-4CB0F8A575E8}"/>
+    <workbookView xWindow="4820" yWindow="460" windowWidth="17160" windowHeight="16620" xr2:uid="{44B2F2F3-C1F6-DD4A-8564-4CB0F8A575E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>hostStatus</t>
   </si>
@@ -72,19 +72,34 @@
     <t>IB</t>
   </si>
   <si>
-    <t>31663_7#1000</t>
-  </si>
-  <si>
-    <t>1234STDY1234</t>
-  </si>
-  <si>
-    <t>SAMPLE</t>
-  </si>
-  <si>
     <t>submittingInstitution</t>
   </si>
   <si>
     <t>Wellcome Sanger Institute</t>
+  </si>
+  <si>
+    <t>1234STDY1235</t>
+  </si>
+  <si>
+    <t>NOLANEID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   MENINGITIS   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   31663_7#1000   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1234STDY1234   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   SAMPLE   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   IB   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Wellcome Sanger Institute       </t>
   </si>
 </sst>
 </file>
@@ -446,7 +461,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,7 +489,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -494,7 +509,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -514,27 +529,44 @@
         <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added missing  e2e scenario
</commit_message>
<xml_diff>
--- a/e2e/fixtures/test_committable.xlsx
+++ b/e2e/fixtures/test_committable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kp11/workspace/applications/monocle/e2e/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B039AD-65B1-214C-AE64-1BF674D5F24B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63831E77-9D0B-AD48-9A38-7117FBB9622E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="460" windowWidth="17160" windowHeight="16620" xr2:uid="{44B2F2F3-C1F6-DD4A-8564-4CB0F8A575E8}"/>
+    <workbookView xWindow="4820" yWindow="460" windowWidth="17160" windowHeight="16580" xr2:uid="{44B2F2F3-C1F6-DD4A-8564-4CB0F8A575E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>hostStatus</t>
   </si>
@@ -81,9 +81,6 @@
     <t>1234STDY1235</t>
   </si>
   <si>
-    <t>NOLANEID</t>
-  </si>
-  <si>
     <t xml:space="preserve">   MENINGITIS   </t>
   </si>
   <si>
@@ -100,6 +97,15 @@
   </si>
   <si>
     <t xml:space="preserve">       Wellcome Sanger Institute       </t>
+  </si>
+  <si>
+    <t>1234STDY1236</t>
+  </si>
+  <si>
+    <t>NOLANEID1</t>
+  </si>
+  <si>
+    <t>NOLANEID2</t>
   </si>
 </sst>
 </file>
@@ -461,7 +467,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,22 +540,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -560,12 +566,29 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>